<commit_message>
Please enter the commit message for your changes. Lines starting 	new file:   Curi Temp/.ipynb_checkpoints/QUINCKE'S METHOD-checkpoint.ipynb
</commit_message>
<xml_diff>
--- a/Forbidden energy gap/feg.xlsx
+++ b/Forbidden energy gap/feg.xlsx
@@ -32,8 +32,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -100,12 +101,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -129,7 +134,7 @@
   <dimension ref="A1:F95"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -149,11 +154,11 @@
       <c r="B2" s="1" t="n">
         <v>0.11</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="2" t="n">
         <f aca="false">MOD(B2,0.02)/0.002</f>
         <v>5</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="2" t="n">
         <f aca="false">MOD(A2,20)</f>
         <v>5</v>
       </c>
@@ -165,11 +170,11 @@
       <c r="B3" s="1" t="n">
         <v>0.12</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="2" t="n">
         <f aca="false">MOD(B3,0.02)/0.002</f>
         <v>0</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="2" t="n">
         <f aca="false">MOD(A3,20)</f>
         <v>0</v>
       </c>
@@ -181,11 +186,11 @@
       <c r="B4" s="1" t="n">
         <v>0.14</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="2" t="n">
         <f aca="false">MOD(B4,0.02)/0.002</f>
         <v>0</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="2" t="n">
         <f aca="false">MOD(A4,20)</f>
         <v>15</v>
       </c>
@@ -197,11 +202,11 @@
       <c r="B5" s="1" t="n">
         <v>0.15</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="2" t="n">
         <f aca="false">MOD(B5,0.02)/0.002</f>
         <v>4.99999999999999</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="2" t="n">
         <f aca="false">MOD(A5,20)</f>
         <v>10</v>
       </c>
@@ -213,11 +218,11 @@
       <c r="B6" s="1" t="n">
         <v>0.16</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="2" t="n">
         <f aca="false">MOD(B6,0.02)/0.002</f>
         <v>0</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="2" t="n">
         <f aca="false">MOD(A6,20)</f>
         <v>5</v>
       </c>
@@ -229,11 +234,11 @@
       <c r="B7" s="1" t="n">
         <v>0.17</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="2" t="n">
         <f aca="false">MOD(B7,0.02)/0.002</f>
         <v>5</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="2" t="n">
         <f aca="false">MOD(A7,20)</f>
         <v>0</v>
       </c>
@@ -245,11 +250,11 @@
       <c r="B8" s="1" t="n">
         <v>0.18</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="2" t="n">
         <f aca="false">MOD(B8,0.02)/0.002</f>
         <v>0</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="2" t="n">
         <f aca="false">MOD(A8,20)</f>
         <v>15</v>
       </c>
@@ -261,11 +266,11 @@
       <c r="B9" s="1" t="n">
         <v>0.2</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="2" t="n">
         <f aca="false">MOD(B9,0.02)/0.002</f>
         <v>0</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="2" t="n">
         <f aca="false">MOD(A9,20)</f>
         <v>10</v>
       </c>
@@ -277,11 +282,11 @@
       <c r="B10" s="1" t="n">
         <v>0.21</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="2" t="n">
         <f aca="false">MOD(B10,0.02)/0.002</f>
         <v>4.99999999999999</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="2" t="n">
         <f aca="false">MOD(A10,20)</f>
         <v>5</v>
       </c>
@@ -293,11 +298,11 @@
       <c r="B11" s="1" t="n">
         <v>0.22</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="2" t="n">
         <f aca="false">MOD(B11,0.02)/0.002</f>
         <v>0</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11" s="2" t="n">
         <f aca="false">MOD(A11,20)</f>
         <v>0</v>
       </c>
@@ -309,11 +314,11 @@
       <c r="B12" s="1" t="n">
         <v>0.23</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="2" t="n">
         <f aca="false">MOD(B12,0.02)/0.002</f>
         <v>5</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12" s="2" t="n">
         <f aca="false">MOD(A12,20)</f>
         <v>15</v>
       </c>
@@ -325,11 +330,11 @@
       <c r="B13" s="1" t="n">
         <v>0.25</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="2" t="n">
         <f aca="false">MOD(B13,0.02)/0.002</f>
         <v>5</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F13" s="2" t="n">
         <f aca="false">MOD(A13,20)</f>
         <v>10</v>
       </c>
@@ -341,11 +346,11 @@
       <c r="B14" s="1" t="n">
         <v>0.26</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="2" t="n">
         <f aca="false">MOD(B14,0.02)/0.002</f>
         <v>0</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14" s="2" t="n">
         <f aca="false">MOD(A14,20)</f>
         <v>5</v>
       </c>
@@ -357,11 +362,11 @@
       <c r="B15" s="1" t="n">
         <v>0.27</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="2" t="n">
         <f aca="false">MOD(B15,0.02)/0.002</f>
         <v>5</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F15" s="2" t="n">
         <f aca="false">MOD(A15,20)</f>
         <v>0</v>
       </c>
@@ -373,11 +378,11 @@
       <c r="B16" s="1" t="n">
         <v>0.29</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="2" t="n">
         <f aca="false">MOD(B16,0.02)/0.002</f>
         <v>4.99999999999998</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="F16" s="2" t="n">
         <f aca="false">MOD(A16,20)</f>
         <v>15</v>
       </c>
@@ -389,11 +394,11 @@
       <c r="B17" s="1" t="n">
         <v>0.3</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="2" t="n">
         <f aca="false">MOD(B17,0.02)/0.002</f>
         <v>0</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="F17" s="2" t="n">
         <f aca="false">MOD(A17,20)</f>
         <v>10</v>
       </c>
@@ -405,11 +410,11 @@
       <c r="B18" s="1" t="n">
         <v>0.31</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="D18" s="2" t="n">
         <f aca="false">MOD(B18,0.02)/0.002</f>
         <v>5</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="F18" s="2" t="n">
         <f aca="false">MOD(A18,20)</f>
         <v>5</v>
       </c>
@@ -421,11 +426,11 @@
       <c r="B19" s="1" t="n">
         <v>0.32</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="2" t="n">
         <f aca="false">MOD(B19,0.02)/0.002</f>
         <v>0</v>
       </c>
-      <c r="F19" s="0" t="n">
+      <c r="F19" s="2" t="n">
         <f aca="false">MOD(A19,20)</f>
         <v>0</v>
       </c>
@@ -437,11 +442,11 @@
       <c r="B20" s="1" t="n">
         <v>0.34</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="D20" s="2" t="n">
         <f aca="false">MOD(B20,0.02)/0.002</f>
         <v>0</v>
       </c>
-      <c r="F20" s="0" t="n">
+      <c r="F20" s="2" t="n">
         <f aca="false">MOD(A20,20)</f>
         <v>15</v>
       </c>
@@ -453,11 +458,11 @@
       <c r="B21" s="1" t="n">
         <v>0.35</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D21" s="2" t="n">
         <f aca="false">MOD(B21,0.02)/0.002</f>
         <v>4.99999999999998</v>
       </c>
-      <c r="F21" s="0" t="n">
+      <c r="F21" s="2" t="n">
         <f aca="false">MOD(A21,20)</f>
         <v>10</v>
       </c>
@@ -469,11 +474,11 @@
       <c r="B22" s="1" t="n">
         <v>0.36</v>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="D22" s="2" t="n">
         <f aca="false">MOD(B22,0.02)/0.002</f>
         <v>0</v>
       </c>
-      <c r="F22" s="0" t="n">
+      <c r="F22" s="2" t="n">
         <f aca="false">MOD(A22,20)</f>
         <v>5</v>
       </c>

</xml_diff>